<commit_message>
minimal scaffold for linux work
</commit_message>
<xml_diff>
--- a/tmBBsplay/rnd1_splayBBs.xlsx
+++ b/tmBBsplay/rnd1_splayBBs.xlsx
@@ -1,16 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="176" firstSheet="0" activeTab="0"/>
+    <workbookView minimized="1" xWindow="0" yWindow="1760" windowWidth="19000" windowHeight="13240" tabRatio="176"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -248,30 +252,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -283,7 +269,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -291,1867 +277,2157 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="100000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="66.6836734693878"/>
-    <col collapsed="false" hidden="false" max="8" min="2" style="0" width="24.8112244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
+    <col min="1" max="1" width="57.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2">
         <v>256</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2">
         <v>207</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2">
         <v>112</v>
       </c>
-      <c r="E2" s="0" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="F2" s="0" t="n">
+      <c r="E2">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="F2">
         <v>6.5</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2">
         <v>5</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="H2">
         <v>12.57</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3">
         <v>155</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3">
         <v>114</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3">
         <v>126</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3">
         <v>4</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3">
         <v>6.2</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3">
         <v>4.2</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="H3">
         <v>12.89</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4">
         <v>150</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4">
         <v>152</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4">
         <v>126</v>
       </c>
-      <c r="E4" s="0" t="n">
-        <v>4.1</v>
-      </c>
-      <c r="F4" s="0" t="n">
+      <c r="E4">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="F4">
         <v>6.2</v>
       </c>
-      <c r="G4" s="0" t="n">
-        <v>4.1</v>
-      </c>
-      <c r="H4" s="0" t="n">
+      <c r="G4">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="H4">
         <v>12.91</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5">
         <v>137</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5">
         <v>189</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5">
         <v>126</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5">
         <v>4.2</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5">
         <v>6.2</v>
       </c>
-      <c r="G5" s="0" t="n">
-        <v>4.1</v>
-      </c>
-      <c r="H5" s="0" t="n">
+      <c r="G5">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="H5">
         <v>12.92</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6">
         <v>109</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6">
         <v>241</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6">
         <v>126</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6">
         <v>4.5</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6">
         <v>6.2</v>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="G6">
         <v>4</v>
       </c>
-      <c r="H6" s="0" t="n">
+      <c r="H6">
         <v>12.97</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7">
         <v>119</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7">
         <v>387</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7">
         <v>130</v>
       </c>
-      <c r="E7" s="0" t="n">
-        <v>5.9</v>
-      </c>
-      <c r="F7" s="0" t="n">
+      <c r="E7">
+        <v>5.9</v>
+      </c>
+      <c r="F7">
         <v>6.1</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="G7">
         <v>5.6</v>
       </c>
-      <c r="H7" s="0" t="n">
+      <c r="H7">
         <v>12.98</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8">
         <v>143</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8">
         <v>364</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8">
         <v>134</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8">
         <v>5.8</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="F8">
         <v>6.1</v>
       </c>
-      <c r="G8" s="0" t="n">
-        <v>5.9</v>
-      </c>
-      <c r="H8" s="0" t="n">
+      <c r="G8">
+        <v>5.9</v>
+      </c>
+      <c r="H8">
         <v>13</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9">
         <v>115</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9">
         <v>137</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9">
         <v>106</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9">
         <v>5.7</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="F9">
         <v>7.2</v>
       </c>
-      <c r="G9" s="0" t="n">
+      <c r="G9">
         <v>5.6</v>
       </c>
-      <c r="H9" s="0" t="n">
+      <c r="H9">
         <v>13.02</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10">
         <v>151</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10">
         <v>361</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10">
         <v>102</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10">
         <v>6</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="F10">
         <v>6.3</v>
       </c>
-      <c r="G10" s="0" t="n">
-        <v>5.9</v>
-      </c>
-      <c r="H10" s="0" t="n">
+      <c r="G10">
+        <v>5.9</v>
+      </c>
+      <c r="H10">
         <v>13.03</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11">
         <v>182</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11">
         <v>135</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11">
         <v>106</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11">
         <v>5.6</v>
       </c>
-      <c r="F11" s="0" t="n">
+      <c r="F11">
         <v>7.2</v>
       </c>
-      <c r="G11" s="0" t="n">
+      <c r="G11">
         <v>5.7</v>
       </c>
-      <c r="H11" s="0" t="n">
+      <c r="H11">
         <v>13.03</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12">
         <v>103</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12">
         <v>585</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="D12">
         <v>120</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E12">
         <v>5.8</v>
       </c>
-      <c r="F12" s="0" t="n">
+      <c r="F12">
         <v>5.7</v>
       </c>
-      <c r="G12" s="0" t="n">
-        <v>5.9</v>
-      </c>
-      <c r="H12" s="0" t="n">
+      <c r="G12">
+        <v>5.9</v>
+      </c>
+      <c r="H12">
         <v>13.03</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B13">
         <v>241</v>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="C13">
         <v>126</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="D13">
         <v>102</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="E13">
         <v>5.6</v>
       </c>
-      <c r="F13" s="0" t="n">
+      <c r="F13">
         <v>7.2</v>
       </c>
-      <c r="G13" s="0" t="n">
-        <v>5.9</v>
-      </c>
-      <c r="H13" s="0" t="n">
+      <c r="G13">
+        <v>5.9</v>
+      </c>
+      <c r="H13">
         <v>13.04</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="0" t="n">
+      <c r="B14">
         <v>111</v>
       </c>
-      <c r="C14" s="0" t="n">
+      <c r="C14">
         <v>336</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="D14">
         <v>134</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="E14">
         <v>5.8</v>
       </c>
-      <c r="F14" s="0" t="n">
+      <c r="F14">
         <v>6.1</v>
       </c>
-      <c r="G14" s="0" t="n">
+      <c r="G14">
         <v>6</v>
       </c>
-      <c r="H14" s="0" t="n">
+      <c r="H14">
         <v>13.04</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="0" t="n">
+      <c r="B15">
         <v>152</v>
       </c>
-      <c r="C15" s="0" t="n">
+      <c r="C15">
         <v>551</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="D15">
         <v>122</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="E15">
         <v>5.7</v>
       </c>
-      <c r="F15" s="0" t="n">
+      <c r="F15">
         <v>5.7</v>
       </c>
-      <c r="G15" s="0" t="n">
+      <c r="G15">
         <v>5.8</v>
       </c>
-      <c r="H15" s="0" t="n">
+      <c r="H15">
         <v>13.05</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="0" t="n">
+      <c r="B16">
         <v>249</v>
       </c>
-      <c r="C16" s="0" t="n">
+      <c r="C16">
         <v>501</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="D16">
         <v>134</v>
       </c>
-      <c r="E16" s="0" t="n">
+      <c r="E16">
         <v>5.6</v>
       </c>
-      <c r="F16" s="0" t="n">
+      <c r="F16">
         <v>5.8</v>
       </c>
-      <c r="G16" s="0" t="n">
-        <v>5.9</v>
-      </c>
-      <c r="H16" s="0" t="n">
+      <c r="G16">
+        <v>5.9</v>
+      </c>
+      <c r="H16">
         <v>13.1</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+    <row r="17" spans="1:8">
+      <c r="A17" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="0" t="n">
+      <c r="B17">
         <v>126</v>
       </c>
-      <c r="C17" s="0" t="n">
+      <c r="C17">
         <v>401</v>
       </c>
-      <c r="D17" s="0" t="n">
+      <c r="D17">
         <v>140</v>
       </c>
-      <c r="E17" s="0" t="n">
+      <c r="E17">
         <v>5.6</v>
       </c>
-      <c r="F17" s="0" t="n">
-        <v>5.9</v>
-      </c>
-      <c r="G17" s="0" t="n">
-        <v>5.9</v>
-      </c>
-      <c r="H17" s="0" t="n">
+      <c r="F17">
+        <v>5.9</v>
+      </c>
+      <c r="G17">
+        <v>5.9</v>
+      </c>
+      <c r="H17">
         <v>13.11</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="0" t="n">
+      <c r="B18">
         <v>406</v>
       </c>
-      <c r="C18" s="0" t="n">
+      <c r="C18">
         <v>463</v>
       </c>
-      <c r="D18" s="0" t="n">
+      <c r="D18">
         <v>114</v>
       </c>
-      <c r="E18" s="0" t="n">
+      <c r="E18">
         <v>5.6</v>
       </c>
-      <c r="F18" s="0" t="n">
+      <c r="F18">
         <v>5.7</v>
       </c>
-      <c r="G18" s="0" t="n">
-        <v>5.9</v>
-      </c>
-      <c r="H18" s="0" t="n">
+      <c r="G18">
+        <v>5.9</v>
+      </c>
+      <c r="H18">
         <v>13.12</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="0" t="n">
+      <c r="B19">
         <v>406</v>
       </c>
-      <c r="C19" s="0" t="n">
+      <c r="C19">
         <v>463</v>
       </c>
-      <c r="D19" s="0" t="n">
+      <c r="D19">
         <v>114</v>
       </c>
-      <c r="E19" s="0" t="n">
+      <c r="E19">
         <v>5.6</v>
       </c>
-      <c r="F19" s="0" t="n">
+      <c r="F19">
         <v>5.7</v>
       </c>
-      <c r="G19" s="0" t="n">
-        <v>5.9</v>
-      </c>
-      <c r="H19" s="0" t="n">
+      <c r="G19">
+        <v>5.9</v>
+      </c>
+      <c r="H19">
         <v>13.12</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="0" t="n">
+      <c r="B20">
         <v>119</v>
       </c>
-      <c r="C20" s="0" t="n">
+      <c r="C20">
         <v>249</v>
       </c>
-      <c r="D20" s="0" t="n">
+      <c r="D20">
         <v>104</v>
       </c>
-      <c r="E20" s="0" t="n">
-        <v>5.9</v>
-      </c>
-      <c r="F20" s="0" t="n">
+      <c r="E20">
+        <v>5.9</v>
+      </c>
+      <c r="F20">
         <v>6.3</v>
       </c>
-      <c r="G20" s="0" t="n">
-        <v>5.9</v>
-      </c>
-      <c r="H20" s="0" t="n">
+      <c r="G20">
+        <v>5.9</v>
+      </c>
+      <c r="H20">
         <v>13.14</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+    <row r="21" spans="1:8">
+      <c r="A21" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="0" t="n">
+      <c r="B21">
         <v>119</v>
       </c>
-      <c r="C21" s="0" t="n">
+      <c r="C21">
         <v>249</v>
       </c>
-      <c r="D21" s="0" t="n">
+      <c r="D21">
         <v>104</v>
       </c>
-      <c r="E21" s="0" t="n">
-        <v>5.9</v>
-      </c>
-      <c r="F21" s="0" t="n">
+      <c r="E21">
+        <v>5.9</v>
+      </c>
+      <c r="F21">
         <v>6.3</v>
       </c>
-      <c r="G21" s="0" t="n">
-        <v>5.9</v>
-      </c>
-      <c r="H21" s="0" t="n">
+      <c r="G21">
+        <v>5.9</v>
+      </c>
+      <c r="H21">
         <v>13.14</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+    <row r="22" spans="1:8">
+      <c r="A22" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="0" t="n">
+      <c r="B22">
         <v>165</v>
       </c>
-      <c r="C22" s="0" t="n">
+      <c r="C22">
         <v>235</v>
       </c>
-      <c r="D22" s="0" t="n">
+      <c r="D22">
         <v>136</v>
       </c>
-      <c r="E22" s="0" t="n">
+      <c r="E22">
         <v>5.6</v>
       </c>
-      <c r="F22" s="0" t="n">
+      <c r="F22">
         <v>6.1</v>
       </c>
-      <c r="G22" s="0" t="n">
-        <v>5.9</v>
-      </c>
-      <c r="H22" s="0" t="n">
+      <c r="G22">
+        <v>5.9</v>
+      </c>
+      <c r="H22">
         <v>13.14</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+    <row r="23" spans="1:8">
+      <c r="A23" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="0" t="n">
+      <c r="B23">
         <v>330</v>
       </c>
-      <c r="C23" s="0" t="n">
+      <c r="C23">
         <v>465</v>
       </c>
-      <c r="D23" s="0" t="n">
+      <c r="D23">
         <v>134</v>
       </c>
-      <c r="E23" s="0" t="n">
+      <c r="E23">
         <v>5.6</v>
       </c>
-      <c r="F23" s="0" t="n">
+      <c r="F23">
         <v>5.8</v>
       </c>
-      <c r="G23" s="0" t="n">
+      <c r="G23">
         <v>6</v>
       </c>
-      <c r="H23" s="0" t="n">
+      <c r="H23">
         <v>13.15</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+    <row r="24" spans="1:8">
+      <c r="A24" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="0" t="n">
+      <c r="B24">
         <v>233</v>
       </c>
-      <c r="C24" s="0" t="n">
+      <c r="C24">
         <v>356</v>
       </c>
-      <c r="D24" s="0" t="n">
+      <c r="D24">
         <v>140</v>
       </c>
-      <c r="E24" s="0" t="n">
+      <c r="E24">
         <v>5.6</v>
       </c>
-      <c r="F24" s="0" t="n">
-        <v>5.9</v>
-      </c>
-      <c r="G24" s="0" t="n">
+      <c r="F24">
+        <v>5.9</v>
+      </c>
+      <c r="G24">
         <v>6</v>
       </c>
-      <c r="H24" s="0" t="n">
+      <c r="H24">
         <v>13.15</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+    <row r="25" spans="1:8">
+      <c r="A25" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="0" t="n">
+      <c r="B25">
         <v>233</v>
       </c>
-      <c r="C25" s="0" t="n">
+      <c r="C25">
         <v>356</v>
       </c>
-      <c r="D25" s="0" t="n">
+      <c r="D25">
         <v>140</v>
       </c>
-      <c r="E25" s="0" t="n">
+      <c r="E25">
         <v>5.6</v>
       </c>
-      <c r="F25" s="0" t="n">
-        <v>5.9</v>
-      </c>
-      <c r="G25" s="0" t="n">
+      <c r="F25">
+        <v>5.9</v>
+      </c>
+      <c r="G25">
         <v>6</v>
       </c>
-      <c r="H25" s="0" t="n">
+      <c r="H25">
         <v>13.15</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+    <row r="26" spans="1:8">
+      <c r="A26" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="0" t="n">
+      <c r="B26">
         <v>328</v>
       </c>
-      <c r="C26" s="0" t="n">
+      <c r="C26">
         <v>285</v>
       </c>
-      <c r="D26" s="0" t="n">
+      <c r="D26">
         <v>555</v>
       </c>
-      <c r="E26" s="0" t="n">
+      <c r="E26">
         <v>5.8</v>
       </c>
-      <c r="F26" s="0" t="n">
+      <c r="F26">
         <v>6.2</v>
       </c>
-      <c r="G26" s="0" t="n">
+      <c r="G26">
         <v>6</v>
       </c>
-      <c r="H26" s="0" t="n">
+      <c r="H26">
         <v>13.26</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+    <row r="27" spans="1:8">
+      <c r="A27" t="s">
         <v>33</v>
       </c>
-      <c r="B27" s="0" t="n">
+      <c r="B27">
         <v>155</v>
       </c>
-      <c r="C27" s="0" t="n">
+      <c r="C27">
         <v>140</v>
       </c>
-      <c r="D27" s="0" t="n">
+      <c r="D27">
         <v>558</v>
       </c>
-      <c r="E27" s="0" t="n">
+      <c r="E27">
         <v>5.8</v>
       </c>
-      <c r="F27" s="0" t="n">
+      <c r="F27">
         <v>6</v>
       </c>
-      <c r="G27" s="0" t="n">
-        <v>5.9</v>
-      </c>
-      <c r="H27" s="0" t="n">
+      <c r="G27">
+        <v>5.9</v>
+      </c>
+      <c r="H27">
         <v>13.26</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+    <row r="28" spans="1:8">
+      <c r="A28" t="s">
         <v>34</v>
       </c>
-      <c r="B28" s="0" t="n">
+      <c r="B28">
         <v>236</v>
       </c>
-      <c r="C28" s="0" t="n">
+      <c r="C28">
         <v>153</v>
       </c>
-      <c r="D28" s="0" t="n">
+      <c r="D28">
         <v>590</v>
       </c>
-      <c r="E28" s="0" t="n">
+      <c r="E28">
         <v>5.8</v>
       </c>
-      <c r="F28" s="0" t="n">
+      <c r="F28">
         <v>6.2</v>
       </c>
-      <c r="G28" s="0" t="n">
-        <v>5.9</v>
-      </c>
-      <c r="H28" s="0" t="n">
+      <c r="G28">
+        <v>5.9</v>
+      </c>
+      <c r="H28">
         <v>13.26</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+    <row r="29" spans="1:8">
+      <c r="A29" t="s">
         <v>35</v>
       </c>
-      <c r="B29" s="0" t="n">
+      <c r="B29">
         <v>117</v>
       </c>
-      <c r="C29" s="0" t="n">
+      <c r="C29">
         <v>148</v>
       </c>
-      <c r="D29" s="0" t="n">
+      <c r="D29">
         <v>296</v>
       </c>
-      <c r="E29" s="0" t="n">
-        <v>5.9</v>
-      </c>
-      <c r="F29" s="0" t="n">
+      <c r="E29">
+        <v>5.9</v>
+      </c>
+      <c r="F29">
         <v>6.5</v>
       </c>
-      <c r="G29" s="0" t="n">
-        <v>5.9</v>
-      </c>
-      <c r="H29" s="0" t="n">
+      <c r="G29">
+        <v>5.9</v>
+      </c>
+      <c r="H29">
         <v>13.27</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+    <row r="30" spans="1:8">
+      <c r="A30" t="s">
         <v>36</v>
       </c>
-      <c r="B30" s="0" t="n">
+      <c r="B30">
         <v>190</v>
       </c>
-      <c r="C30" s="0" t="n">
+      <c r="C30">
         <v>106</v>
       </c>
-      <c r="D30" s="0" t="n">
+      <c r="D30">
         <v>326</v>
       </c>
-      <c r="E30" s="0" t="n">
+      <c r="E30">
         <v>5.8</v>
       </c>
-      <c r="F30" s="0" t="n">
+      <c r="F30">
         <v>6.5</v>
       </c>
-      <c r="G30" s="0" t="n">
-        <v>5.9</v>
-      </c>
-      <c r="H30" s="0" t="n">
+      <c r="G30">
+        <v>5.9</v>
+      </c>
+      <c r="H30">
         <v>13.27</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+    <row r="31" spans="1:8">
+      <c r="A31" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="0" t="n">
+      <c r="B31">
         <v>126</v>
       </c>
-      <c r="C31" s="0" t="n">
+      <c r="C31">
         <v>150</v>
       </c>
-      <c r="D31" s="0" t="n">
+      <c r="D31">
         <v>514</v>
       </c>
-      <c r="E31" s="0" t="n">
-        <v>5.9</v>
-      </c>
-      <c r="F31" s="0" t="n">
+      <c r="E31">
+        <v>5.9</v>
+      </c>
+      <c r="F31">
         <v>5.8</v>
       </c>
-      <c r="G31" s="0" t="n">
-        <v>5.9</v>
-      </c>
-      <c r="H31" s="0" t="n">
+      <c r="G31">
+        <v>5.9</v>
+      </c>
+      <c r="H31">
         <v>13.27</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+    <row r="32" spans="1:8">
+      <c r="A32" t="s">
         <v>38</v>
       </c>
-      <c r="B32" s="0" t="n">
+      <c r="B32">
         <v>280</v>
       </c>
-      <c r="C32" s="0" t="n">
+      <c r="C32">
         <v>132</v>
       </c>
-      <c r="D32" s="0" t="n">
+      <c r="D32">
         <v>304</v>
       </c>
-      <c r="E32" s="0" t="n">
+      <c r="E32">
         <v>5.8</v>
       </c>
-      <c r="F32" s="0" t="n">
+      <c r="F32">
         <v>6.4</v>
       </c>
-      <c r="G32" s="0" t="n">
-        <v>5.9</v>
-      </c>
-      <c r="H32" s="0" t="n">
+      <c r="G32">
+        <v>5.9</v>
+      </c>
+      <c r="H32">
         <v>13.28</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+    <row r="33" spans="1:8">
+      <c r="A33" t="s">
         <v>39</v>
       </c>
-      <c r="B33" s="0" t="n">
+      <c r="B33">
         <v>224</v>
       </c>
-      <c r="C33" s="0" t="n">
+      <c r="C33">
         <v>118</v>
       </c>
-      <c r="D33" s="0" t="n">
+      <c r="D33">
         <v>118</v>
       </c>
-      <c r="E33" s="0" t="n">
+      <c r="E33">
         <v>4.2</v>
       </c>
-      <c r="F33" s="0" t="n">
+      <c r="F33">
         <v>6.6</v>
       </c>
-      <c r="G33" s="0" t="n">
-        <v>4.4</v>
-      </c>
-      <c r="H33" s="0" t="n">
+      <c r="G33">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="H33">
         <v>13.29</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+    <row r="34" spans="1:8">
+      <c r="A34" t="s">
         <v>40</v>
       </c>
-      <c r="B34" s="0" t="n">
+      <c r="B34">
         <v>352</v>
       </c>
-      <c r="C34" s="0" t="n">
+      <c r="C34">
         <v>202</v>
       </c>
-      <c r="D34" s="0" t="n">
+      <c r="D34">
         <v>280</v>
       </c>
-      <c r="E34" s="0" t="n">
+      <c r="E34">
         <v>5.8</v>
       </c>
-      <c r="F34" s="0" t="n">
+      <c r="F34">
         <v>6.4</v>
       </c>
-      <c r="G34" s="0" t="n">
+      <c r="G34">
         <v>6</v>
       </c>
-      <c r="H34" s="0" t="n">
+      <c r="H34">
         <v>13.29</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+    <row r="35" spans="1:8">
+      <c r="A35" t="s">
         <v>41</v>
       </c>
-      <c r="B35" s="0" t="n">
+      <c r="B35">
         <v>107</v>
       </c>
-      <c r="C35" s="0" t="n">
+      <c r="C35">
         <v>122</v>
       </c>
-      <c r="D35" s="0" t="n">
+      <c r="D35">
         <v>350</v>
       </c>
-      <c r="E35" s="0" t="n">
+      <c r="E35">
         <v>6</v>
       </c>
-      <c r="F35" s="0" t="n">
+      <c r="F35">
         <v>6.3</v>
       </c>
-      <c r="G35" s="0" t="n">
+      <c r="G35">
         <v>5.7</v>
       </c>
-      <c r="H35" s="0" t="n">
+      <c r="H35">
         <v>13.29</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+    <row r="36" spans="1:8">
+      <c r="A36" t="s">
         <v>42</v>
       </c>
-      <c r="B36" s="0" t="n">
+      <c r="B36">
         <v>439</v>
       </c>
-      <c r="C36" s="0" t="n">
+      <c r="C36">
         <v>371</v>
       </c>
-      <c r="D36" s="0" t="n">
+      <c r="D36">
         <v>252</v>
       </c>
-      <c r="E36" s="0" t="n">
+      <c r="E36">
         <v>6</v>
       </c>
-      <c r="F36" s="0" t="n">
+      <c r="F36">
         <v>6.3</v>
       </c>
-      <c r="G36" s="0" t="n">
+      <c r="G36">
         <v>6</v>
       </c>
-      <c r="H36" s="0" t="n">
+      <c r="H36">
         <v>13.3</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+    <row r="37" spans="1:8">
+      <c r="A37" t="s">
         <v>43</v>
       </c>
-      <c r="B37" s="0" t="n">
+      <c r="B37">
         <v>112</v>
       </c>
-      <c r="C37" s="0" t="n">
+      <c r="C37">
         <v>143</v>
       </c>
-      <c r="D37" s="0" t="n">
+      <c r="D37">
         <v>100</v>
       </c>
-      <c r="E37" s="0" t="n">
+      <c r="E37">
         <v>4.2</v>
       </c>
-      <c r="F37" s="0" t="n">
+      <c r="F37">
         <v>6.8</v>
       </c>
-      <c r="G37" s="0" t="n">
-        <v>4.1</v>
-      </c>
-      <c r="H37" s="0" t="n">
+      <c r="G37">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="H37">
         <v>13.31</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+    <row r="38" spans="1:8">
+      <c r="A38" t="s">
         <v>44</v>
       </c>
-      <c r="B38" s="0" t="n">
+      <c r="B38">
         <v>105</v>
       </c>
-      <c r="C38" s="0" t="n">
+      <c r="C38">
         <v>165</v>
       </c>
-      <c r="D38" s="0" t="n">
+      <c r="D38">
         <v>100</v>
       </c>
-      <c r="E38" s="0" t="n">
+      <c r="E38">
         <v>4.3</v>
       </c>
-      <c r="F38" s="0" t="n">
+      <c r="F38">
         <v>6.8</v>
       </c>
-      <c r="G38" s="0" t="n">
+      <c r="G38">
         <v>4</v>
       </c>
-      <c r="H38" s="0" t="n">
+      <c r="H38">
         <v>13.31</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+    <row r="39" spans="1:8">
+      <c r="A39" t="s">
         <v>45</v>
       </c>
-      <c r="B39" s="0" t="n">
+      <c r="B39">
         <v>196</v>
       </c>
-      <c r="C39" s="0" t="n">
+      <c r="C39">
         <v>204</v>
       </c>
-      <c r="D39" s="0" t="n">
+      <c r="D39">
         <v>118</v>
       </c>
-      <c r="E39" s="0" t="n">
-        <v>4.4</v>
-      </c>
-      <c r="F39" s="0" t="n">
+      <c r="E39">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="F39">
         <v>6.6</v>
       </c>
-      <c r="G39" s="0" t="n">
-        <v>4.4</v>
-      </c>
-      <c r="H39" s="0" t="n">
+      <c r="G39">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="H39">
         <v>13.32</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+    <row r="40" spans="1:8">
+      <c r="A40" t="s">
         <v>46</v>
       </c>
-      <c r="B40" s="0" t="n">
+      <c r="B40">
         <v>245</v>
       </c>
-      <c r="C40" s="0" t="n">
+      <c r="C40">
         <v>325</v>
       </c>
-      <c r="D40" s="0" t="n">
+      <c r="D40">
         <v>128</v>
       </c>
-      <c r="E40" s="0" t="n">
+      <c r="E40">
         <v>6</v>
       </c>
-      <c r="F40" s="0" t="n">
+      <c r="F40">
         <v>6.2</v>
       </c>
-      <c r="G40" s="0" t="n">
-        <v>5.9</v>
-      </c>
-      <c r="H40" s="0" t="n">
+      <c r="G40">
+        <v>5.9</v>
+      </c>
+      <c r="H40">
         <v>13.33</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+    <row r="41" spans="1:8">
+      <c r="A41" t="s">
         <v>47</v>
       </c>
-      <c r="B41" s="0" t="n">
+      <c r="B41">
         <v>167</v>
       </c>
-      <c r="C41" s="0" t="n">
+      <c r="C41">
         <v>255</v>
       </c>
-      <c r="D41" s="0" t="n">
+      <c r="D41">
         <v>100</v>
       </c>
-      <c r="E41" s="0" t="n">
+      <c r="E41">
         <v>6</v>
       </c>
-      <c r="F41" s="0" t="n">
+      <c r="F41">
         <v>6.4</v>
       </c>
-      <c r="G41" s="0" t="n">
+      <c r="G41">
         <v>5.6</v>
       </c>
-      <c r="H41" s="0" t="n">
+      <c r="H41">
         <v>13.34</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+    <row r="42" spans="1:8">
+      <c r="A42" t="s">
         <v>48</v>
       </c>
-      <c r="B42" s="0" t="n">
+      <c r="B42">
         <v>182</v>
       </c>
-      <c r="C42" s="0" t="n">
+      <c r="C42">
         <v>239</v>
       </c>
-      <c r="D42" s="0" t="n">
+      <c r="D42">
         <v>118</v>
       </c>
-      <c r="E42" s="0" t="n">
+      <c r="E42">
         <v>4.5</v>
       </c>
-      <c r="F42" s="0" t="n">
+      <c r="F42">
         <v>6.6</v>
       </c>
-      <c r="G42" s="0" t="n">
+      <c r="G42">
         <v>4.3</v>
       </c>
-      <c r="H42" s="0" t="n">
+      <c r="H42">
         <v>13.34</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+    <row r="43" spans="1:8">
+      <c r="A43" t="s">
         <v>49</v>
       </c>
-      <c r="B43" s="0" t="n">
+      <c r="B43">
         <v>167</v>
       </c>
-      <c r="C43" s="0" t="n">
+      <c r="C43">
         <v>214</v>
       </c>
-      <c r="D43" s="0" t="n">
+      <c r="D43">
         <v>150</v>
       </c>
-      <c r="E43" s="0" t="n">
-        <v>5.9</v>
-      </c>
-      <c r="F43" s="0" t="n">
+      <c r="E43">
+        <v>5.9</v>
+      </c>
+      <c r="F43">
         <v>6.3</v>
       </c>
-      <c r="G43" s="0" t="n">
+      <c r="G43">
         <v>5.8</v>
       </c>
-      <c r="H43" s="0" t="n">
+      <c r="H43">
         <v>13.34</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+    <row r="44" spans="1:8">
+      <c r="A44" t="s">
         <v>50</v>
       </c>
-      <c r="B44" s="0" t="n">
+      <c r="B44">
         <v>165</v>
       </c>
-      <c r="C44" s="0" t="n">
+      <c r="C44">
         <v>263</v>
       </c>
-      <c r="D44" s="0" t="n">
+      <c r="D44">
         <v>118</v>
       </c>
-      <c r="E44" s="0" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="F44" s="0" t="n">
+      <c r="E44">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="F44">
         <v>6.6</v>
       </c>
-      <c r="G44" s="0" t="n">
+      <c r="G44">
         <v>4.3</v>
       </c>
-      <c r="H44" s="0" t="n">
+      <c r="H44">
         <v>13.36</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+    <row r="45" spans="1:8">
+      <c r="A45" t="s">
         <v>51</v>
       </c>
-      <c r="B45" s="0" t="n">
+      <c r="B45">
         <v>165</v>
       </c>
-      <c r="C45" s="0" t="n">
+      <c r="C45">
         <v>263</v>
       </c>
-      <c r="D45" s="0" t="n">
+      <c r="D45">
         <v>118</v>
       </c>
-      <c r="E45" s="0" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="F45" s="0" t="n">
+      <c r="E45">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="F45">
         <v>6.6</v>
       </c>
-      <c r="G45" s="0" t="n">
+      <c r="G45">
         <v>4.3</v>
       </c>
-      <c r="H45" s="0" t="n">
+      <c r="H45">
         <v>13.36</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+    <row r="46" spans="1:8">
+      <c r="A46" t="s">
         <v>52</v>
       </c>
-      <c r="B46" s="0" t="n">
+      <c r="B46">
         <v>106</v>
       </c>
-      <c r="C46" s="0" t="n">
+      <c r="C46">
         <v>100</v>
       </c>
-      <c r="D46" s="0" t="n">
+      <c r="D46">
         <v>106</v>
       </c>
-      <c r="E46" s="0" t="n">
+      <c r="E46">
         <v>5.7</v>
       </c>
-      <c r="F46" s="0" t="n">
+      <c r="F46">
         <v>6.1</v>
       </c>
-      <c r="G46" s="0" t="n">
+      <c r="G46">
         <v>6</v>
       </c>
-      <c r="H46" s="0" t="n">
+      <c r="H46">
         <v>13.39</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+    <row r="47" spans="1:8">
+      <c r="A47" t="s">
         <v>53</v>
       </c>
-      <c r="B47" s="0" t="n">
+      <c r="B47">
         <v>111</v>
       </c>
-      <c r="C47" s="0" t="n">
+      <c r="C47">
         <v>543</v>
       </c>
-      <c r="D47" s="0" t="n">
+      <c r="D47">
         <v>110</v>
       </c>
-      <c r="E47" s="0" t="n">
+      <c r="E47">
         <v>6</v>
       </c>
-      <c r="F47" s="0" t="n">
+      <c r="F47">
         <v>6</v>
       </c>
-      <c r="G47" s="0" t="n">
+      <c r="G47">
         <v>6</v>
       </c>
-      <c r="H47" s="0" t="n">
+      <c r="H47">
         <v>13.43</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+    <row r="48" spans="1:8">
+      <c r="A48" t="s">
         <v>54</v>
       </c>
-      <c r="B48" s="0" t="n">
+      <c r="B48">
         <v>120</v>
       </c>
-      <c r="C48" s="0" t="n">
+      <c r="C48">
         <v>106</v>
       </c>
-      <c r="D48" s="0" t="n">
+      <c r="D48">
         <v>114</v>
       </c>
-      <c r="E48" s="0" t="n">
+      <c r="E48">
         <v>5.2</v>
       </c>
-      <c r="F48" s="0" t="n">
+      <c r="F48">
         <v>7.1</v>
       </c>
-      <c r="G48" s="0" t="n">
-        <v>4.9</v>
-      </c>
-      <c r="H48" s="0" t="n">
+      <c r="G48">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="H48">
         <v>13.67</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
+    <row r="49" spans="1:8">
+      <c r="A49" t="s">
         <v>55</v>
       </c>
-      <c r="B49" s="0" t="n">
+      <c r="B49">
         <v>117</v>
       </c>
-      <c r="C49" s="0" t="n">
+      <c r="C49">
         <v>116</v>
       </c>
-      <c r="D49" s="0" t="n">
+      <c r="D49">
         <v>114</v>
       </c>
-      <c r="E49" s="0" t="n">
+      <c r="E49">
         <v>5.2</v>
       </c>
-      <c r="F49" s="0" t="n">
+      <c r="F49">
         <v>7.1</v>
       </c>
-      <c r="G49" s="0" t="n">
-        <v>4.9</v>
-      </c>
-      <c r="H49" s="0" t="n">
+      <c r="G49">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="H49">
         <v>13.68</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
+    <row r="50" spans="1:8">
+      <c r="A50" t="s">
         <v>56</v>
       </c>
-      <c r="B50" s="0" t="n">
+      <c r="B50">
         <v>110</v>
       </c>
-      <c r="C50" s="0" t="n">
+      <c r="C50">
         <v>139</v>
       </c>
-      <c r="D50" s="0" t="n">
+      <c r="D50">
         <v>114</v>
       </c>
-      <c r="E50" s="0" t="n">
+      <c r="E50">
         <v>5.2</v>
       </c>
-      <c r="F50" s="0" t="n">
+      <c r="F50">
         <v>7.1</v>
       </c>
-      <c r="G50" s="0" t="n">
-        <v>4.9</v>
-      </c>
-      <c r="H50" s="0" t="n">
+      <c r="G50">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="H50">
         <v>13.68</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
+    <row r="51" spans="1:8">
+      <c r="A51" t="s">
         <v>57</v>
       </c>
-      <c r="B51" s="0" t="n">
+      <c r="B51">
         <v>292</v>
       </c>
-      <c r="C51" s="0" t="n">
+      <c r="C51">
         <v>112</v>
       </c>
-      <c r="D51" s="0" t="n">
+      <c r="D51">
         <v>100</v>
       </c>
-      <c r="E51" s="0" t="n">
+      <c r="E51">
         <v>4.3</v>
       </c>
-      <c r="F51" s="0" t="n">
+      <c r="F51">
         <v>6.9</v>
       </c>
-      <c r="G51" s="0" t="n">
+      <c r="G51">
         <v>4.7</v>
       </c>
-      <c r="H51" s="0" t="n">
+      <c r="H51">
         <v>13.7</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
+    <row r="52" spans="1:8">
+      <c r="A52" t="s">
         <v>58</v>
       </c>
-      <c r="B52" s="0" t="n">
+      <c r="B52">
         <v>292</v>
       </c>
-      <c r="C52" s="0" t="n">
+      <c r="C52">
         <v>112</v>
       </c>
-      <c r="D52" s="0" t="n">
+      <c r="D52">
         <v>100</v>
       </c>
-      <c r="E52" s="0" t="n">
+      <c r="E52">
         <v>4.3</v>
       </c>
-      <c r="F52" s="0" t="n">
+      <c r="F52">
         <v>6.9</v>
       </c>
-      <c r="G52" s="0" t="n">
+      <c r="G52">
         <v>4.7</v>
       </c>
-      <c r="H52" s="0" t="n">
+      <c r="H52">
         <v>13.7</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
+    <row r="53" spans="1:8">
+      <c r="A53" t="s">
         <v>59</v>
       </c>
-      <c r="B53" s="0" t="n">
+      <c r="B53">
         <v>281</v>
       </c>
-      <c r="C53" s="0" t="n">
+      <c r="C53">
         <v>159</v>
       </c>
-      <c r="D53" s="0" t="n">
+      <c r="D53">
         <v>100</v>
       </c>
-      <c r="E53" s="0" t="n">
-        <v>4.4</v>
-      </c>
-      <c r="F53" s="0" t="n">
+      <c r="E53">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="F53">
         <v>6.9</v>
       </c>
-      <c r="G53" s="0" t="n">
+      <c r="G53">
         <v>4.7</v>
       </c>
-      <c r="H53" s="0" t="n">
+      <c r="H53">
         <v>13.71</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
+    <row r="54" spans="1:8">
+      <c r="A54" t="s">
         <v>60</v>
       </c>
-      <c r="B54" s="0" t="n">
+      <c r="B54">
         <v>281</v>
       </c>
-      <c r="C54" s="0" t="n">
+      <c r="C54">
         <v>159</v>
       </c>
-      <c r="D54" s="0" t="n">
+      <c r="D54">
         <v>100</v>
       </c>
-      <c r="E54" s="0" t="n">
-        <v>4.4</v>
-      </c>
-      <c r="F54" s="0" t="n">
+      <c r="E54">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="F54">
         <v>6.9</v>
       </c>
-      <c r="G54" s="0" t="n">
+      <c r="G54">
         <v>4.7</v>
       </c>
-      <c r="H54" s="0" t="n">
+      <c r="H54">
         <v>13.71</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
+    <row r="55" spans="1:8">
+      <c r="A55" t="s">
         <v>61</v>
       </c>
-      <c r="B55" s="0" t="n">
+      <c r="B55">
         <v>261</v>
       </c>
-      <c r="C55" s="0" t="n">
+      <c r="C55">
         <v>206</v>
       </c>
-      <c r="D55" s="0" t="n">
+      <c r="D55">
         <v>100</v>
       </c>
-      <c r="E55" s="0" t="n">
+      <c r="E55">
         <v>4.5</v>
       </c>
-      <c r="F55" s="0" t="n">
+      <c r="F55">
         <v>6.9</v>
       </c>
-      <c r="G55" s="0" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="H55" s="0" t="n">
+      <c r="G55">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="H55">
         <v>13.72</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
+    <row r="56" spans="1:8">
+      <c r="A56" t="s">
         <v>62</v>
       </c>
-      <c r="B56" s="0" t="n">
+      <c r="B56">
         <v>249</v>
       </c>
-      <c r="C56" s="0" t="n">
+      <c r="C56">
         <v>259</v>
       </c>
-      <c r="D56" s="0" t="n">
+      <c r="D56">
         <v>100</v>
       </c>
-      <c r="E56" s="0" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="F56" s="0" t="n">
+      <c r="E56">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="F56">
         <v>6.9</v>
       </c>
-      <c r="G56" s="0" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="H56" s="0" t="n">
+      <c r="G56">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="H56">
         <v>13.73</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
+    <row r="57" spans="1:8">
+      <c r="A57" t="s">
         <v>63</v>
       </c>
-      <c r="B57" s="0" t="n">
+      <c r="B57">
         <v>240</v>
       </c>
-      <c r="C57" s="0" t="n">
+      <c r="C57">
         <v>295</v>
       </c>
-      <c r="D57" s="0" t="n">
+      <c r="D57">
         <v>100</v>
       </c>
-      <c r="E57" s="0" t="n">
+      <c r="E57">
         <v>4.7</v>
       </c>
-      <c r="F57" s="0" t="n">
+      <c r="F57">
         <v>6.9</v>
       </c>
-      <c r="G57" s="0" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="H57" s="0" t="n">
+      <c r="G57">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="H57">
         <v>13.75</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
+    <row r="58" spans="1:8">
+      <c r="A58" t="s">
         <v>64</v>
       </c>
-      <c r="B58" s="0" t="n">
+      <c r="B58">
         <v>218</v>
       </c>
-      <c r="C58" s="0" t="n">
+      <c r="C58">
         <v>315</v>
       </c>
-      <c r="D58" s="0" t="n">
+      <c r="D58">
         <v>100</v>
       </c>
-      <c r="E58" s="0" t="n">
+      <c r="E58">
         <v>4.8</v>
       </c>
-      <c r="F58" s="0" t="n">
+      <c r="F58">
         <v>6.9</v>
       </c>
-      <c r="G58" s="0" t="n">
+      <c r="G58">
         <v>4.5</v>
       </c>
-      <c r="H58" s="0" t="n">
+      <c r="H58">
         <v>13.77</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
+    <row r="59" spans="1:8">
+      <c r="A59" t="s">
         <v>65</v>
       </c>
-      <c r="B59" s="0" t="n">
+      <c r="B59">
         <v>199</v>
       </c>
-      <c r="C59" s="0" t="n">
+      <c r="C59">
         <v>341</v>
       </c>
-      <c r="D59" s="0" t="n">
+      <c r="D59">
         <v>100</v>
       </c>
-      <c r="E59" s="0" t="n">
+      <c r="E59">
         <v>5</v>
       </c>
-      <c r="F59" s="0" t="n">
+      <c r="F59">
         <v>6.9</v>
       </c>
-      <c r="G59" s="0" t="n">
+      <c r="G59">
         <v>4.5</v>
       </c>
-      <c r="H59" s="0" t="n">
+      <c r="H59">
         <v>13.79</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
+    <row r="60" spans="1:8">
+      <c r="A60" t="s">
         <v>66</v>
       </c>
-      <c r="B60" s="0" t="n">
+      <c r="B60">
         <v>179</v>
       </c>
-      <c r="C60" s="0" t="n">
+      <c r="C60">
         <v>352</v>
       </c>
-      <c r="D60" s="0" t="n">
+      <c r="D60">
         <v>100</v>
       </c>
-      <c r="E60" s="0" t="n">
-        <v>5.1</v>
-      </c>
-      <c r="F60" s="0" t="n">
+      <c r="E60">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="F60">
         <v>6.9</v>
       </c>
-      <c r="G60" s="0" t="n">
+      <c r="G60">
         <v>4.5</v>
       </c>
-      <c r="H60" s="0" t="n">
+      <c r="H60">
         <v>13.81</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="s">
+    <row r="61" spans="1:8">
+      <c r="A61" t="s">
         <v>67</v>
       </c>
-      <c r="B61" s="0" t="n">
+      <c r="B61">
         <v>164</v>
       </c>
-      <c r="C61" s="0" t="n">
+      <c r="C61">
         <v>353</v>
       </c>
-      <c r="D61" s="0" t="n">
+      <c r="D61">
         <v>100</v>
       </c>
-      <c r="E61" s="0" t="n">
+      <c r="E61">
         <v>5.2</v>
       </c>
-      <c r="F61" s="0" t="n">
+      <c r="F61">
         <v>6.9</v>
       </c>
-      <c r="G61" s="0" t="n">
-        <v>4.4</v>
-      </c>
-      <c r="H61" s="0" t="n">
+      <c r="G61">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="H61">
         <v>13.83</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
+    <row r="62" spans="1:8">
+      <c r="A62" t="s">
         <v>68</v>
       </c>
-      <c r="B62" s="0" t="n">
+      <c r="B62">
         <v>144</v>
       </c>
-      <c r="C62" s="0" t="n">
+      <c r="C62">
         <v>347</v>
       </c>
-      <c r="D62" s="0" t="n">
+      <c r="D62">
         <v>100</v>
       </c>
-      <c r="E62" s="0" t="n">
+      <c r="E62">
         <v>5.2</v>
       </c>
-      <c r="F62" s="0" t="n">
+      <c r="F62">
         <v>6.9</v>
       </c>
-      <c r="G62" s="0" t="n">
-        <v>4.4</v>
-      </c>
-      <c r="H62" s="0" t="n">
+      <c r="G62">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="H62">
         <v>13.86</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
+    <row r="63" spans="1:8">
+      <c r="A63" t="s">
         <v>69</v>
       </c>
-      <c r="B63" s="0" t="n">
+      <c r="B63">
         <v>153</v>
       </c>
-      <c r="C63" s="0" t="n">
+      <c r="C63">
         <v>101</v>
       </c>
-      <c r="D63" s="0" t="n">
+      <c r="D63">
         <v>118</v>
       </c>
-      <c r="E63" s="0" t="n">
+      <c r="E63">
         <v>5.3</v>
       </c>
-      <c r="F63" s="0" t="n">
+      <c r="F63">
         <v>7.5</v>
       </c>
-      <c r="G63" s="0" t="n">
-        <v>5.1</v>
-      </c>
-      <c r="H63" s="0" t="n">
+      <c r="G63">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="H63">
         <v>14.09</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
+    <row r="64" spans="1:8">
+      <c r="A64" t="s">
         <v>70</v>
       </c>
-      <c r="B64" s="0" t="n">
+      <c r="B64">
         <v>141</v>
       </c>
-      <c r="C64" s="0" t="n">
+      <c r="C64">
         <v>139</v>
       </c>
-      <c r="D64" s="0" t="n">
+      <c r="D64">
         <v>118</v>
       </c>
-      <c r="E64" s="0" t="n">
+      <c r="E64">
         <v>5.4</v>
       </c>
-      <c r="F64" s="0" t="n">
+      <c r="F64">
         <v>7.5</v>
       </c>
-      <c r="G64" s="0" t="n">
-        <v>5.1</v>
-      </c>
-      <c r="H64" s="0" t="n">
+      <c r="G64">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="H64">
         <v>14.1</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="s">
+    <row r="65" spans="1:8">
+      <c r="A65" t="s">
         <v>71</v>
       </c>
-      <c r="B65" s="0" t="n">
+      <c r="B65">
         <v>132</v>
       </c>
-      <c r="C65" s="0" t="n">
+      <c r="C65">
         <v>156</v>
       </c>
-      <c r="D65" s="0" t="n">
+      <c r="D65">
         <v>118</v>
       </c>
-      <c r="E65" s="0" t="n">
+      <c r="E65">
         <v>5.4</v>
       </c>
-      <c r="F65" s="0" t="n">
+      <c r="F65">
         <v>7.5</v>
       </c>
-      <c r="G65" s="0" t="n">
-        <v>5.1</v>
-      </c>
-      <c r="H65" s="0" t="n">
+      <c r="G65">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="H65">
         <v>14.11</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
+    <row r="66" spans="1:8">
+      <c r="A66" t="s">
         <v>72</v>
       </c>
-      <c r="B66" s="0" t="n">
+      <c r="B66">
         <v>125</v>
       </c>
-      <c r="C66" s="0" t="n">
+      <c r="C66">
         <v>163</v>
       </c>
-      <c r="D66" s="0" t="n">
+      <c r="D66">
         <v>118</v>
       </c>
-      <c r="E66" s="0" t="n">
+      <c r="E66">
         <v>5.4</v>
       </c>
-      <c r="F66" s="0" t="n">
+      <c r="F66">
         <v>7.5</v>
       </c>
-      <c r="G66" s="0" t="n">
-        <v>5.1</v>
-      </c>
-      <c r="H66" s="0" t="n">
+      <c r="G66">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="H66">
         <v>14.11</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
+    <row r="67" spans="1:8">
+      <c r="A67" t="s">
         <v>73</v>
       </c>
-      <c r="B67" s="0" t="n">
+      <c r="B67">
         <v>111</v>
       </c>
-      <c r="C67" s="0" t="n">
+      <c r="C67">
         <v>164</v>
       </c>
-      <c r="D67" s="0" t="n">
+      <c r="D67">
         <v>118</v>
       </c>
-      <c r="E67" s="0" t="n">
+      <c r="E67">
         <v>5.2</v>
       </c>
-      <c r="F67" s="0" t="n">
+      <c r="F67">
         <v>7.5</v>
       </c>
-      <c r="G67" s="0" t="n">
+      <c r="G67">
         <v>5</v>
       </c>
-      <c r="H67" s="0" t="n">
+      <c r="H67">
         <v>14.12</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="s">
+    <row r="68" spans="1:8">
+      <c r="A68" t="s">
         <v>74</v>
       </c>
-      <c r="B68" s="0" t="n">
+      <c r="B68">
         <v>120</v>
       </c>
-      <c r="C68" s="0" t="n">
+      <c r="C68">
         <v>166</v>
       </c>
-      <c r="D68" s="0" t="n">
+      <c r="D68">
         <v>118</v>
       </c>
-      <c r="E68" s="0" t="n">
+      <c r="E68">
         <v>5.3</v>
       </c>
-      <c r="F68" s="0" t="n">
+      <c r="F68">
         <v>7.5</v>
       </c>
-      <c r="G68" s="0" t="n">
-        <v>5.1</v>
-      </c>
-      <c r="H68" s="0" t="n">
+      <c r="G68">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="H68">
         <v>14.12</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="s">
+    <row r="69" spans="1:8">
+      <c r="A69" t="s">
         <v>75</v>
       </c>
-      <c r="B69" s="0" t="n">
+      <c r="B69">
         <v>104</v>
       </c>
-      <c r="C69" s="0" t="n">
+      <c r="C69">
         <v>157</v>
       </c>
-      <c r="D69" s="0" t="n">
+      <c r="D69">
         <v>118</v>
       </c>
-      <c r="E69" s="0" t="n">
-        <v>5.1</v>
-      </c>
-      <c r="F69" s="0" t="n">
+      <c r="E69">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="F69">
         <v>7.5</v>
       </c>
-      <c r="G69" s="0" t="n">
+      <c r="G69">
         <v>5</v>
       </c>
-      <c r="H69" s="0" t="n">
+      <c r="H69">
         <v>14.13</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>